<commit_message>
add basic combo system
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\Documents\My Games\Terraria\ModLoader\Mod Sources\Overdone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaap-Jan\Documents\My Games\Terraria\ModLoader\Mod Sources\Overdone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B850F5-34D1-4C0F-8690-7A671A0A37B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5345D8-3605-45B7-B557-8CBF07B079B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46440" yWindow="2355" windowWidth="30360" windowHeight="18645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of items" sheetId="1" r:id="rId1"/>
@@ -746,17 +746,18 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Apollo Bow and Sharur sprite
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\Documents\My Games\Terraria\ModLoader\Mod Sources\Overdone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7899C1-31EC-44C9-9F0B-B748E89E5058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE450D8B-951B-4F7C-A6D3-BAB9D4E756DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8145" yWindow="2250" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="197">
   <si>
     <t>Mythology</t>
   </si>
@@ -679,9 +679,6 @@
     <t>Melee</t>
   </si>
   <si>
-    <t>Neptune's trident</t>
-  </si>
-  <si>
     <t>Neptune</t>
   </si>
   <si>
@@ -698,6 +695,18 @@
   </si>
   <si>
     <t>Sun; Justice</t>
+  </si>
+  <si>
+    <t>Poseidons trident</t>
+  </si>
+  <si>
+    <t>Neptunes trident</t>
+  </si>
+  <si>
+    <t>Poseidon</t>
+  </si>
+  <si>
+    <t>Hero</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,13 +1331,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
         <v>67</v>
@@ -1389,7 +1398,7 @@
         <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1425,6 +1434,7 @@
       <c r="D29" t="s">
         <v>184</v>
       </c>
+      <c r="E29" s="5"/>
       <c r="F29" t="s">
         <v>19</v>
       </c>
@@ -1491,6 +1501,7 @@
       <c r="D35" t="s">
         <v>98</v>
       </c>
+      <c r="E35" s="5"/>
       <c r="F35" t="s">
         <v>19</v>
       </c>
@@ -1830,13 +1841,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B54" t="s">
         <v>141</v>
       </c>
       <c r="C54" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D54" t="s">
         <v>58</v>
@@ -1876,6 +1887,10 @@
       <c r="D59" t="s">
         <v>62</v>
       </c>
+      <c r="E59" s="5"/>
+      <c r="F59" t="s">
+        <v>19</v>
+      </c>
       <c r="G59" t="s">
         <v>149</v>
       </c>
@@ -1942,11 +1957,32 @@
       <c r="C62" t="s">
         <v>181</v>
       </c>
+      <c r="D62" t="s">
+        <v>196</v>
+      </c>
       <c r="F62" t="s">
         <v>19</v>
       </c>
       <c r="G62" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2057,12 +2093,12 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>